<commit_message>
updated cv and references
</commit_message>
<xml_diff>
--- a/public/files/Formidling.xlsx
+++ b/public/files/Formidling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/st06810/Dropbox/UiB/blog/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A546C3-EC7C-B74E-9181-B3CCBD3B2792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD35756-67E5-4F46-A032-CD05BA41CAFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="47360" windowHeight="18760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2017'!$A$2:$AD$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Ark2'!$B$1:$H$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Ark2'!$B$1:$H$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="337">
   <si>
     <t>p</t>
   </si>
@@ -971,12 +971,6 @@
     <t>Norhordaland regionråd</t>
   </si>
   <si>
-    <t>Samfunnspsykologi</t>
-  </si>
-  <si>
-    <t>Spesialisering i Samfunnspsykologi for psykologer</t>
-  </si>
-  <si>
     <t>Norsk Psykologforening</t>
   </si>
   <si>
@@ -1059,6 +1053,12 @@
   </si>
   <si>
     <t>Barne- og familiedpartementet</t>
+  </si>
+  <si>
+    <t>Spesialistprogram i Samfunnspsykologi</t>
+  </si>
+  <si>
+    <t>Epidemiologi og samfunnspsykologi</t>
   </si>
 </sst>
 </file>
@@ -4712,10 +4712,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4754,59 +4754,59 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>2020</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>251</v>
+        <v>298</v>
       </c>
       <c r="E2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="F2" t="s">
         <v>335</v>
       </c>
       <c r="G2" t="s">
-        <v>336</v>
+        <v>307</v>
       </c>
       <c r="H2">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F3" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="H3">
-        <v>150</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <v>2019</v>
@@ -4818,7 +4818,7 @@
         <v>246</v>
       </c>
       <c r="E4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F4" t="s">
         <v>329</v>
@@ -4827,154 +4827,154 @@
         <v>330</v>
       </c>
       <c r="H4">
-        <v>10</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B5">
         <v>2019</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>324</v>
+        <v>271</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>318</v>
+        <v>246</v>
       </c>
       <c r="E5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G5" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H5">
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>2019</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="E6" t="s">
+        <v>323</v>
+      </c>
+      <c r="F6" t="s">
         <v>324</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>318</v>
-      </c>
-      <c r="E6" t="s">
-        <v>322</v>
-      </c>
-      <c r="F6" t="s">
-        <v>323</v>
-      </c>
       <c r="G6" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>2019</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G7" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="H7">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>2019</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>264</v>
+        <v>322</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>252</v>
+        <v>316</v>
       </c>
       <c r="E8" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F8" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="G8" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="H8">
-        <v>1200</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <v>2019</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E9" t="s">
         <v>312</v>
       </c>
       <c r="F9" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H9">
-        <v>350</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>2019</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>296</v>
+        <v>251</v>
       </c>
       <c r="E10" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F10" t="s">
         <v>308</v>
@@ -4983,12 +4983,12 @@
         <v>309</v>
       </c>
       <c r="H10">
-        <v>30</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11">
         <v>2019</v>
@@ -5000,102 +5000,101 @@
         <v>296</v>
       </c>
       <c r="E11" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="F11" t="s">
-        <v>305</v>
+        <v>335</v>
       </c>
       <c r="G11" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H11">
-        <v>150</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12">
         <v>2019</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="E12" t="s">
+        <v>311</v>
+      </c>
+      <c r="F12" t="s">
+        <v>305</v>
+      </c>
+      <c r="G12" t="s">
+        <v>306</v>
+      </c>
+      <c r="H12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>2019</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="E12" t="s">
-        <v>316</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E13" t="s">
+        <v>314</v>
+      </c>
+      <c r="F13" t="s">
         <v>106</v>
       </c>
-      <c r="G12" t="s">
-        <v>317</v>
-      </c>
-      <c r="H12">
+      <c r="G13" t="s">
+        <v>315</v>
+      </c>
+      <c r="H13">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20">
-      <c r="A13">
-        <f>ROWS(B13:B59)</f>
+    <row r="14" spans="1:8" ht="20">
+      <c r="A14">
+        <f>ROWS(B14:B60)</f>
         <v>47</v>
-      </c>
-      <c r="B13">
-        <v>2018</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>291</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>292</v>
-      </c>
-      <c r="G13" t="s">
-        <v>293</v>
-      </c>
-      <c r="H13">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16">
-      <c r="A14">
-        <f>A13-1</f>
-        <v>46</v>
       </c>
       <c r="B14">
         <v>2018</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>289</v>
+        <v>244</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>292</v>
       </c>
       <c r="G14" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="H14">
-        <v>25</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16">
       <c r="A15">
-        <f t="shared" ref="A15:A59" si="0">A14-1</f>
-        <v>45</v>
+        <f>A14-1</f>
+        <v>46</v>
       </c>
       <c r="B15">
         <v>2018</v>
@@ -5106,104 +5105,104 @@
       <c r="D15" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="F15" t="s">
-        <v>286</v>
+      <c r="E15" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>289</v>
       </c>
       <c r="G15" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="H15">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16">
       <c r="A16">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <f t="shared" ref="A16:A60" si="0">A15-1</f>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>2018</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E16" t="s">
-        <v>283</v>
+        <v>252</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>288</v>
       </c>
       <c r="F16" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G16" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="H16">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>2018</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>296</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F17" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G17" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="H17">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>2018</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>247</v>
+        <v>296</v>
       </c>
       <c r="E18" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F18" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="G18" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="H18">
-        <v>150</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>2018</v>
@@ -5215,103 +5214,103 @@
         <v>247</v>
       </c>
       <c r="E19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F19" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G19" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="H19">
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16">
+    <row r="20" spans="1:8">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>2018</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>260</v>
+        <v>247</v>
+      </c>
+      <c r="E20" t="s">
+        <v>276</v>
       </c>
       <c r="F20" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="G20" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="H20">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="E21" t="s">
-        <v>257</v>
+        <v>297</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>260</v>
       </c>
       <c r="F21" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="G21" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="H21">
-        <v>800</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>2017</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E22" t="s">
-        <v>130</v>
+        <v>257</v>
       </c>
       <c r="F22" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G22" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
       <c r="H22">
-        <v>20</v>
+        <v>800</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>2017</v>
@@ -5323,76 +5322,76 @@
         <v>252</v>
       </c>
       <c r="E23" t="s">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="F23" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="G23" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="H23">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24">
         <v>2017</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>298</v>
+        <v>252</v>
       </c>
       <c r="E24" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="F24" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="G24" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="H24">
-        <v>200</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25">
         <v>2017</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>251</v>
+        <v>298</v>
       </c>
       <c r="E25" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="F25" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="G25" t="s">
-        <v>34</v>
+        <v>200</v>
       </c>
       <c r="H25">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26">
         <v>2017</v>
@@ -5404,76 +5403,76 @@
         <v>251</v>
       </c>
       <c r="E26" t="s">
-        <v>301</v>
+        <v>192</v>
       </c>
       <c r="F26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G26" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="H26">
-        <v>20</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B27">
         <v>2017</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>147</v>
+        <v>251</v>
       </c>
       <c r="E27" t="s">
-        <v>187</v>
+        <v>301</v>
       </c>
       <c r="F27" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="G27" t="s">
-        <v>188</v>
+        <v>114</v>
       </c>
       <c r="H27">
-        <v>130</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>2017</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>255</v>
+        <v>147</v>
       </c>
       <c r="E28" t="s">
-        <v>259</v>
+        <v>187</v>
       </c>
       <c r="F28" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="G28" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="H28">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>2017</v>
@@ -5485,22 +5484,22 @@
         <v>255</v>
       </c>
       <c r="E29" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
       <c r="F29" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G29" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="H29">
-        <v>70</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>2017</v>
@@ -5512,13 +5511,13 @@
         <v>255</v>
       </c>
       <c r="E30" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F30" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G30" t="s">
-        <v>184</v>
+        <v>114</v>
       </c>
       <c r="H30">
         <v>70</v>
@@ -5527,7 +5526,7 @@
     <row r="31" spans="1:8">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>2017</v>
@@ -5539,49 +5538,49 @@
         <v>255</v>
       </c>
       <c r="E31" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F31" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G31" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H31">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>2017</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>297</v>
+        <v>255</v>
       </c>
       <c r="E32" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="F32" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="G32" t="s">
+        <v>180</v>
+      </c>
+      <c r="H32">
         <v>50</v>
-      </c>
-      <c r="H32">
-        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B33">
         <v>2017</v>
@@ -5593,22 +5592,22 @@
         <v>297</v>
       </c>
       <c r="E33" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F33" t="s">
-        <v>235</v>
+        <v>160</v>
       </c>
       <c r="G33" t="s">
-        <v>163</v>
+        <v>50</v>
       </c>
       <c r="H33">
-        <v>370</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B34">
         <v>2017</v>
@@ -5620,103 +5619,103 @@
         <v>297</v>
       </c>
       <c r="E34" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F34" t="s">
-        <v>167</v>
+        <v>235</v>
       </c>
       <c r="G34" t="s">
-        <v>34</v>
+        <v>163</v>
       </c>
       <c r="H34">
-        <v>30</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B35">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>246</v>
+        <v>297</v>
       </c>
       <c r="E35" t="s">
-        <v>302</v>
+        <v>167</v>
       </c>
       <c r="F35" t="s">
-        <v>98</v>
+        <v>167</v>
       </c>
       <c r="G35" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="H35">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B36">
         <v>2016</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>302</v>
       </c>
       <c r="F36" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G36" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="H36">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B37">
         <v>2016</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="E37" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="G37" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="H37">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B38">
         <v>2016</v>
@@ -5725,25 +5724,25 @@
         <v>264</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>299</v>
+        <v>252</v>
       </c>
       <c r="E38" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="F38" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="G38" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="H38">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B39">
         <v>2016</v>
@@ -5752,124 +5751,124 @@
         <v>264</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>252</v>
+        <v>299</v>
       </c>
       <c r="E39" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F39" t="s">
-        <v>237</v>
+        <v>132</v>
       </c>
       <c r="G39" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H39">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B40">
         <v>2016</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>298</v>
+        <v>252</v>
       </c>
       <c r="E40" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F40" t="s">
-        <v>155</v>
+        <v>237</v>
       </c>
       <c r="G40" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="H40">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B41">
         <v>2016</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>249</v>
+        <v>298</v>
       </c>
       <c r="E41" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="F41" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="G41" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="H41">
-        <v>150</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B42">
         <v>2016</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E42" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F42" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G42" t="s">
         <v>114</v>
       </c>
       <c r="H42">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B43">
         <v>2016</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>147</v>
+        <v>251</v>
       </c>
       <c r="E43" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="F43" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="G43" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="H43">
         <v>100</v>
@@ -5878,34 +5877,34 @@
     <row r="44" spans="1:8">
       <c r="A44">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B44">
         <v>2016</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>296</v>
+        <v>147</v>
       </c>
       <c r="E44" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="F44" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="G44" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
       <c r="H44">
-        <v>40</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B45">
         <v>2016</v>
@@ -5917,49 +5916,49 @@
         <v>296</v>
       </c>
       <c r="E45" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="F45" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="G45" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="H45">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B46">
         <v>2016</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>247</v>
+        <v>296</v>
       </c>
       <c r="E46" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="F46" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="G46" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="H46">
-        <v>300</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B47">
         <v>2016</v>
@@ -5971,49 +5970,49 @@
         <v>247</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="F47" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G47" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="H47">
-        <v>70</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B48">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E48" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="G48" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="H48">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B49">
         <v>2015</v>
@@ -6025,22 +6024,22 @@
         <v>246</v>
       </c>
       <c r="E49" t="s">
-        <v>303</v>
+        <v>16</v>
       </c>
       <c r="F49" t="s">
-        <v>239</v>
+        <v>17</v>
       </c>
       <c r="G49" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="H49">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B50">
         <v>2015</v>
@@ -6055,34 +6054,34 @@
         <v>303</v>
       </c>
       <c r="F50" t="s">
-        <v>56</v>
+        <v>239</v>
       </c>
       <c r="G50" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="H50">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B51">
         <v>2015</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E51" t="s">
-        <v>42</v>
+        <v>303</v>
       </c>
       <c r="F51" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="G51" t="s">
         <v>5</v>
@@ -6094,7 +6093,7 @@
     <row r="52" spans="1:8">
       <c r="A52">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B52">
         <v>2015</v>
@@ -6106,22 +6105,22 @@
         <v>244</v>
       </c>
       <c r="E52" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F52" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G52" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="H52">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B53">
         <v>2015</v>
@@ -6133,10 +6132,10 @@
         <v>244</v>
       </c>
       <c r="E53" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F53" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G53" t="s">
         <v>50</v>
@@ -6148,61 +6147,61 @@
     <row r="54" spans="1:8">
       <c r="A54">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B54">
         <v>2015</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="E54" t="s">
-        <v>304</v>
+        <v>52</v>
       </c>
       <c r="F54" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="G54" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H54">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B55">
         <v>2015</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>147</v>
+        <v>251</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>304</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G55" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H55">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B56">
         <v>2015</v>
@@ -6214,40 +6213,40 @@
         <v>147</v>
       </c>
       <c r="E56" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F56" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="H56">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B57">
         <v>2015</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>247</v>
+        <v>147</v>
       </c>
       <c r="E57" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G57" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H57">
         <v>50</v>
@@ -6256,34 +6255,34 @@
     <row r="58" spans="1:8">
       <c r="A58">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B58">
         <v>2015</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>297</v>
+        <v>247</v>
       </c>
       <c r="E58" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F58" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G58" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="H58">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B59">
         <v>2015</v>
@@ -6298,20 +6297,47 @@
         <v>36</v>
       </c>
       <c r="F59" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G59" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H59">
         <v>80</v>
       </c>
     </row>
+    <row r="60" spans="1:8">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>2015</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="E60" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:H59" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B18:H60">
-    <sortCondition descending="1" ref="B20:B60"/>
-    <sortCondition descending="1" ref="C20:C60"/>
+  <autoFilter ref="B1:H60" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B19:H61">
+    <sortCondition descending="1" ref="B21:B61"/>
+    <sortCondition descending="1" ref="C21:C61"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
small update to blog menus
</commit_message>
<xml_diff>
--- a/public/files/Formidling.xlsx
+++ b/public/files/Formidling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/st06810/Dropbox/UiB/blog/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD35756-67E5-4F46-A032-CD05BA41CAFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE9217D-766C-D74C-86C4-04FEE8B17434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="47360" windowHeight="18760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3340" yWindow="1700" windowWidth="41940" windowHeight="22100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2017'!$A$2:$AD$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Ark2'!$B$1:$H$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Ark2'!$B$1:$I$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="340">
   <si>
     <t>p</t>
   </si>
@@ -821,12 +821,6 @@
     <t>Mnd</t>
   </si>
   <si>
-    <t>En plass i samfunnet</t>
-  </si>
-  <si>
-    <t>Schizofrenidagene</t>
-  </si>
-  <si>
     <t>Levekårsundersøkelsen og tanker om tiltak</t>
   </si>
   <si>
@@ -908,15 +902,6 @@
     <t>RKBU Nord</t>
   </si>
   <si>
-    <t>Septemberkonferansen</t>
-  </si>
-  <si>
-    <t>RVTS Vest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fattigdom og Marginalisering </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ekspertmøte – utfordringsbilete og eigna tiltak utsette barn og unge </t>
   </si>
   <si>
@@ -947,9 +932,6 @@
     <t>aug</t>
   </si>
   <si>
-    <t>ep</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kva veit vi om helse og levekår til utsette barn og unge? </t>
   </si>
   <si>
@@ -1059,6 +1041,33 @@
   </si>
   <si>
     <t>Epidemiologi og samfunnspsykologi</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Presentasjon</t>
+  </si>
+  <si>
+    <t>Online learning in Community Psychology</t>
+  </si>
+  <si>
+    <t>TelEd Panel discussion</t>
+  </si>
+  <si>
+    <t>Department of Education</t>
+  </si>
+  <si>
+    <t>Department meeting</t>
+  </si>
+  <si>
+    <t>Department of psychosocial science</t>
+  </si>
+  <si>
+    <t>Frontrunners meeting</t>
+  </si>
+  <si>
+    <t>UoB</t>
   </si>
 </sst>
 </file>
@@ -1068,9 +1077,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1096,11 +1112,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="KozGoPr6N"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1180,20 +1191,20 @@
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1207,8 +1218,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1217,9 +1228,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Benyttet hyperkobling" xfId="2" builtinId="9" hidden="1"/>
@@ -1514,11 +1526,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
@@ -1528,12 +1540,12 @@
     <col min="7" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1">
+    <row r="6" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +1609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="8" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1629,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="9" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1661,7 +1673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="10" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1693,7 +1705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="11" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="12" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="13" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1789,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1">
+    <row r="14" spans="1:10" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1821,7 +1833,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1">
+    <row r="15" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1853,7 +1865,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1">
+    <row r="16" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1885,7 +1897,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1">
+    <row r="17" spans="1:10" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1930,12 +1942,12 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="13" customFormat="1" ht="48">
+    <row r="1" spans="1:26" s="13" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>59</v>
       </c>
@@ -2015,7 +2027,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" ht="128">
+    <row r="2" spans="1:26" s="13" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -2074,7 +2086,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="13" customFormat="1" ht="160">
+    <row r="3" spans="1:26" s="13" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
@@ -2133,7 +2145,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="13" customFormat="1" ht="48">
+    <row r="4" spans="1:26" s="13" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -2189,7 +2201,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="13" customFormat="1" ht="144">
+    <row r="5" spans="1:26" s="13" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -2245,7 +2257,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="13" customFormat="1" ht="96">
+    <row r="6" spans="1:26" s="13" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
@@ -2301,7 +2313,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" ht="112">
+    <row r="7" spans="1:26" s="13" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>1</v>
       </c>
@@ -2357,7 +2369,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="13" customFormat="1" ht="112">
+    <row r="8" spans="1:26" s="13" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
@@ -2413,7 +2425,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="13" customFormat="1" ht="192">
+    <row r="9" spans="1:26" s="13" customFormat="1" ht="192" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>1</v>
       </c>
@@ -2469,7 +2481,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="13" customFormat="1" ht="112">
+    <row r="10" spans="1:26" s="13" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>1</v>
       </c>
@@ -2525,7 +2537,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="13" customFormat="1" ht="96">
+    <row r="11" spans="1:26" s="13" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>1</v>
       </c>
@@ -2584,7 +2596,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="13" customFormat="1" ht="64">
+    <row r="12" spans="1:26" s="13" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>1</v>
       </c>
@@ -2646,7 +2658,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="13" customFormat="1" ht="80">
+    <row r="13" spans="1:26" s="13" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -2708,7 +2720,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="13" customFormat="1" ht="176">
+    <row r="14" spans="1:26" s="13" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>1</v>
       </c>
@@ -2767,7 +2779,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="13" customFormat="1" ht="160">
+    <row r="15" spans="1:26" s="13" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>1</v>
       </c>
@@ -2840,12 +2852,12 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>213</v>
       </c>
@@ -2910,7 +2922,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2978,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3043,7 +3055,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3105,7 +3117,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3182,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3247,7 +3259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -3306,7 +3318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -3365,7 +3377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -3439,7 +3451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -3507,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3569,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -3643,7 +3655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -3705,7 +3717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -3781,7 +3793,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="16"/>
     <col min="3" max="3" width="92" bestFit="1" customWidth="1"/>
@@ -3789,7 +3801,7 @@
     <col min="5" max="5" width="48.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>231</v>
       </c>
@@ -3809,7 +3821,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3832,7 +3844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -3855,7 +3867,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -3878,7 +3890,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2015</v>
       </c>
@@ -3901,7 +3913,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2015</v>
       </c>
@@ -3924,7 +3936,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3947,7 +3959,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -3970,7 +3982,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -3992,7 +4004,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2015</v>
       </c>
@@ -4015,7 +4027,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -4038,7 +4050,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2015</v>
       </c>
@@ -4061,7 +4073,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -4085,7 +4097,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2016</v>
       </c>
@@ -4109,7 +4121,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2016</v>
       </c>
@@ -4133,7 +4145,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2016</v>
       </c>
@@ -4158,7 +4170,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2016</v>
       </c>
@@ -4182,7 +4194,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2016</v>
       </c>
@@ -4206,7 +4218,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2016</v>
       </c>
@@ -4230,7 +4242,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2016</v>
       </c>
@@ -4252,7 +4264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2016</v>
       </c>
@@ -4276,7 +4288,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2016</v>
       </c>
@@ -4300,7 +4312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2016</v>
       </c>
@@ -4324,7 +4336,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2016</v>
       </c>
@@ -4348,7 +4360,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2016</v>
       </c>
@@ -4371,7 +4383,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2016</v>
       </c>
@@ -4395,7 +4407,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2017</v>
       </c>
@@ -4419,7 +4431,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2017</v>
       </c>
@@ -4443,7 +4455,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2017</v>
       </c>
@@ -4465,7 +4477,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2017</v>
       </c>
@@ -4489,7 +4501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2017</v>
       </c>
@@ -4513,7 +4525,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2017</v>
       </c>
@@ -4537,7 +4549,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2017</v>
       </c>
@@ -4561,7 +4573,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2017</v>
       </c>
@@ -4584,7 +4596,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2017</v>
       </c>
@@ -4607,7 +4619,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2017</v>
       </c>
@@ -4631,7 +4643,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2017</v>
       </c>
@@ -4655,7 +4667,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2017</v>
       </c>
@@ -4679,7 +4691,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2017</v>
       </c>
@@ -4712,29 +4724,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="10.83203125" style="16"/>
-    <col min="5" max="5" width="92" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.33203125" customWidth="1"/>
+    <col min="5" max="5" width="99.5" customWidth="1"/>
+    <col min="6" max="6" width="65.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B1" t="s">
         <v>231</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>256</v>
@@ -4746,154 +4759,172 @@
         <v>234</v>
       </c>
       <c r="G1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H1" t="s">
         <v>218</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>59</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="19">
+        <v>53</v>
+      </c>
+      <c r="B2" s="19">
         <v>2020</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="I2" s="19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="19">
+        <v>52</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="I3" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="19">
+        <v>51</v>
+      </c>
+      <c r="B4" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="I4" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="E5" t="s">
+        <v>330</v>
+      </c>
+      <c r="F5" t="s">
+        <v>329</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>301</v>
+      </c>
+      <c r="I5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>298</v>
-      </c>
-      <c r="E2" t="s">
-        <v>336</v>
-      </c>
-      <c r="F2" t="s">
-        <v>335</v>
-      </c>
-      <c r="G2" t="s">
-        <v>307</v>
-      </c>
-      <c r="H2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>58</v>
-      </c>
-      <c r="B3">
-        <v>2020</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="D6" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E6" t="s">
+        <v>326</v>
+      </c>
+      <c r="F6" t="s">
+        <v>327</v>
+      </c>
+      <c r="G6" t="s">
         <v>332</v>
       </c>
-      <c r="F3" t="s">
-        <v>333</v>
-      </c>
-      <c r="G3" t="s">
-        <v>334</v>
-      </c>
-      <c r="H3">
+      <c r="H6" t="s">
+        <v>328</v>
+      </c>
+      <c r="I6">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>57</v>
-      </c>
-      <c r="B4">
-        <v>2019</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="E4" t="s">
-        <v>329</v>
-      </c>
-      <c r="F4" t="s">
-        <v>329</v>
-      </c>
-      <c r="G4" t="s">
-        <v>330</v>
-      </c>
-      <c r="H4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>56</v>
-      </c>
-      <c r="B5">
-        <v>2019</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="E5" t="s">
-        <v>326</v>
-      </c>
-      <c r="F5" t="s">
-        <v>327</v>
-      </c>
-      <c r="G5" t="s">
-        <v>328</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>55</v>
-      </c>
-      <c r="B6">
-        <v>2019</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>316</v>
-      </c>
-      <c r="E6" t="s">
-        <v>323</v>
-      </c>
-      <c r="F6" t="s">
-        <v>324</v>
-      </c>
-      <c r="G6" t="s">
-        <v>325</v>
-      </c>
-      <c r="H6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B7">
         <v>2019</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>322</v>
+        <v>269</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>316</v>
+        <v>246</v>
       </c>
       <c r="E7" t="s">
         <v>320</v>
@@ -4902,448 +4933,488 @@
         <v>321</v>
       </c>
       <c r="G7" t="s">
-        <v>331</v>
-      </c>
-      <c r="H7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H7" t="s">
+        <v>322</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>2019</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>322</v>
+        <v>269</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>316</v>
+        <v>246</v>
       </c>
       <c r="E8" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="F8" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="G8" t="s">
-        <v>319</v>
-      </c>
-      <c r="H8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H8" t="s">
+        <v>324</v>
+      </c>
+      <c r="I8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <v>2019</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>264</v>
+        <v>316</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>252</v>
+        <v>310</v>
       </c>
       <c r="E9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F9" t="s">
         <v>312</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
         <v>313</v>
       </c>
-      <c r="G9" t="s">
-        <v>307</v>
-      </c>
-      <c r="H9">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>2019</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>268</v>
+        <v>316</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>251</v>
+        <v>310</v>
       </c>
       <c r="E10" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="F10" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="G10" t="s">
-        <v>309</v>
-      </c>
-      <c r="H10">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H10" t="s">
+        <v>325</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>2019</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>270</v>
+        <v>316</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="E11" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="F11" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="G11" t="s">
-        <v>307</v>
-      </c>
-      <c r="H11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H11" t="s">
+        <v>319</v>
+      </c>
+      <c r="I11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>2019</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>296</v>
+        <v>252</v>
       </c>
       <c r="E12" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F12" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G12" t="s">
-        <v>306</v>
-      </c>
-      <c r="H12">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H12" t="s">
+        <v>301</v>
+      </c>
+      <c r="I12">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>2019</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D13" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13" t="s">
+        <v>304</v>
+      </c>
+      <c r="F13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G13" t="s">
+        <v>332</v>
+      </c>
+      <c r="H13" t="s">
+        <v>303</v>
+      </c>
+      <c r="I13">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>2019</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="E14" t="s">
+        <v>305</v>
+      </c>
+      <c r="F14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G14" t="s">
+        <v>332</v>
+      </c>
+      <c r="H14" t="s">
+        <v>300</v>
+      </c>
+      <c r="I14">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>2019</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="E15" t="s">
+        <v>330</v>
+      </c>
+      <c r="F15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>301</v>
+      </c>
+      <c r="I15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>2019</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="E13" t="s">
-        <v>314</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E16" t="s">
+        <v>308</v>
+      </c>
+      <c r="F16" t="s">
         <v>106</v>
       </c>
-      <c r="G13" t="s">
-        <v>315</v>
-      </c>
-      <c r="H13">
+      <c r="G16" t="s">
+        <v>332</v>
+      </c>
+      <c r="H16" t="s">
+        <v>309</v>
+      </c>
+      <c r="I16">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20">
-      <c r="A14">
-        <f>ROWS(B14:B60)</f>
-        <v>47</v>
-      </c>
-      <c r="B14">
-        <v>2018</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>291</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>292</v>
-      </c>
-      <c r="G14" t="s">
-        <v>293</v>
-      </c>
-      <c r="H14">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16">
-      <c r="A15">
-        <f>A14-1</f>
-        <v>46</v>
-      </c>
-      <c r="B15">
-        <v>2018</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="G15" t="s">
-        <v>290</v>
-      </c>
-      <c r="H15">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16">
-      <c r="A16">
-        <f t="shared" ref="A16:A60" si="0">A15-1</f>
-        <v>45</v>
-      </c>
-      <c r="B16">
-        <v>2018</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="F16" t="s">
-        <v>286</v>
-      </c>
-      <c r="G16" t="s">
-        <v>287</v>
-      </c>
-      <c r="H16">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9" ht="20" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>2018</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E17" t="s">
-        <v>283</v>
-      </c>
-      <c r="F17" t="s">
-        <v>284</v>
+        <v>244</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>287</v>
       </c>
       <c r="G17" t="s">
-        <v>285</v>
-      </c>
-      <c r="H17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H17" t="s">
+        <v>288</v>
+      </c>
+      <c r="I17">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f t="shared" si="0"/>
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>2018</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="E18" t="s">
-        <v>280</v>
-      </c>
-      <c r="F18" t="s">
-        <v>281</v>
+        <v>252</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>284</v>
       </c>
       <c r="G18" t="s">
-        <v>282</v>
-      </c>
-      <c r="H18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H18" t="s">
+        <v>285</v>
+      </c>
+      <c r="I18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>2018</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>247</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F19" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="G19" t="s">
-        <v>279</v>
-      </c>
-      <c r="H19">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s">
+        <v>283</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
-        <f t="shared" si="0"/>
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>2018</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="E20" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="F20" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="G20" t="s">
-        <v>275</v>
-      </c>
-      <c r="H20">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="16">
+        <v>332</v>
+      </c>
+      <c r="H20" t="s">
+        <v>280</v>
+      </c>
+      <c r="I20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>2018</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="E21" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="E21" t="s">
+        <v>274</v>
+      </c>
+      <c r="F21" t="s">
+        <v>272</v>
+      </c>
+      <c r="G21" t="s">
+        <v>332</v>
+      </c>
+      <c r="H21" t="s">
+        <v>273</v>
+      </c>
+      <c r="I21">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>2018</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E22" t="s">
+        <v>275</v>
+      </c>
+      <c r="F22" t="s">
+        <v>276</v>
+      </c>
+      <c r="G22" t="s">
+        <v>332</v>
+      </c>
+      <c r="H22" t="s">
+        <v>277</v>
+      </c>
+      <c r="I22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>2018</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="F23" t="s">
+        <v>259</v>
+      </c>
+      <c r="G23" t="s">
+        <v>332</v>
+      </c>
+      <c r="H23" t="s">
         <v>260</v>
       </c>
-      <c r="F21" t="s">
-        <v>261</v>
-      </c>
-      <c r="G21" t="s">
-        <v>262</v>
-      </c>
-      <c r="H21">
+      <c r="I23">
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B22">
-        <v>2017</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="E22" t="s">
-        <v>257</v>
-      </c>
-      <c r="F22" t="s">
-        <v>258</v>
-      </c>
-      <c r="G22" t="s">
-        <v>258</v>
-      </c>
-      <c r="H22">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B23">
-        <v>2017</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E23" t="s">
-        <v>130</v>
-      </c>
-      <c r="F23" t="s">
-        <v>238</v>
-      </c>
-      <c r="G23" t="s">
-        <v>205</v>
-      </c>
-      <c r="H23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <v>2017</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>252</v>
@@ -5355,16 +5426,18 @@
         <v>212</v>
       </c>
       <c r="G24" t="s">
+        <v>332</v>
+      </c>
+      <c r="H24" t="s">
         <v>211</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>2017</v>
@@ -5373,223 +5446,239 @@
         <v>266</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>298</v>
+        <v>251</v>
       </c>
       <c r="E25" t="s">
-        <v>199</v>
+        <v>295</v>
       </c>
       <c r="F25" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="G25" t="s">
-        <v>200</v>
-      </c>
-      <c r="H25">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H25" t="s">
+        <v>114</v>
+      </c>
+      <c r="I25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>2017</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>251</v>
+        <v>147</v>
       </c>
       <c r="E26" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F26" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G26" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H26" t="s">
+        <v>188</v>
+      </c>
+      <c r="I26">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>2017</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E27" t="s">
-        <v>301</v>
+        <v>179</v>
       </c>
       <c r="F27" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="G27" t="s">
-        <v>114</v>
-      </c>
-      <c r="H27">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H27" t="s">
+        <v>180</v>
+      </c>
+      <c r="I27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>2017</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>147</v>
+        <v>255</v>
       </c>
       <c r="E28" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F28" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G28" t="s">
-        <v>188</v>
-      </c>
-      <c r="H28">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H28" t="s">
+        <v>184</v>
+      </c>
+      <c r="I28">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>2017</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>255</v>
       </c>
       <c r="E29" t="s">
-        <v>259</v>
+        <v>176</v>
       </c>
       <c r="F29" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="G29" t="s">
-        <v>171</v>
-      </c>
-      <c r="H29">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H29" t="s">
+        <v>114</v>
+      </c>
+      <c r="I29">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B30">
         <v>2017</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>255</v>
       </c>
       <c r="E30" t="s">
-        <v>176</v>
+        <v>257</v>
       </c>
       <c r="F30" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G30" t="s">
-        <v>114</v>
-      </c>
-      <c r="H30">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H30" t="s">
+        <v>171</v>
+      </c>
+      <c r="I30">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B31">
         <v>2017</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>255</v>
+        <v>292</v>
       </c>
       <c r="E31" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="F31" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="G31" t="s">
-        <v>184</v>
-      </c>
-      <c r="H31">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B32">
         <v>2017</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>255</v>
+        <v>292</v>
       </c>
       <c r="E32" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="F32" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="G32" t="s">
-        <v>180</v>
-      </c>
-      <c r="H32">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H32" t="s">
+        <v>163</v>
+      </c>
+      <c r="I32">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B33">
         <v>2017</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E33" t="s">
         <v>159</v>
@@ -5598,746 +5687,628 @@
         <v>160</v>
       </c>
       <c r="G33" t="s">
+        <v>332</v>
+      </c>
+      <c r="H33" t="s">
         <v>50</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B34">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>297</v>
+        <v>246</v>
       </c>
       <c r="E34" t="s">
-        <v>162</v>
+        <v>296</v>
       </c>
       <c r="F34" t="s">
-        <v>235</v>
+        <v>98</v>
       </c>
       <c r="G34" t="s">
-        <v>163</v>
-      </c>
-      <c r="H34">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H34" t="s">
+        <v>97</v>
+      </c>
+      <c r="I34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B35">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>297</v>
+        <v>252</v>
       </c>
       <c r="E35" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="F35" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="G35" t="s">
-        <v>34</v>
-      </c>
-      <c r="H35">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H35" t="s">
+        <v>140</v>
+      </c>
+      <c r="I35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B36">
         <v>2016</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E36" t="s">
-        <v>302</v>
+        <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="G36" t="s">
-        <v>97</v>
-      </c>
-      <c r="H36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H36" t="s">
+        <v>119</v>
+      </c>
+      <c r="I36">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B37">
         <v>2016</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>244</v>
+        <v>293</v>
       </c>
       <c r="E37" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="F37" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="G37" t="s">
-        <v>90</v>
-      </c>
-      <c r="H37">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H37" t="s">
+        <v>154</v>
+      </c>
+      <c r="I37">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B38">
         <v>2016</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F38" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
-      </c>
-      <c r="H38">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I38">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B39">
         <v>2016</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="E39" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F39" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G39" t="s">
-        <v>131</v>
-      </c>
-      <c r="H39">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B40">
         <v>2016</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>252</v>
+        <v>291</v>
       </c>
       <c r="E40" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="F40" t="s">
-        <v>237</v>
+        <v>128</v>
       </c>
       <c r="G40" t="s">
-        <v>140</v>
-      </c>
-      <c r="H40">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H40" t="s">
+        <v>105</v>
+      </c>
+      <c r="I40">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B41">
         <v>2016</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E41" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="F41" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="G41" t="s">
-        <v>154</v>
-      </c>
-      <c r="H41">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H41" t="s">
+        <v>50</v>
+      </c>
+      <c r="I41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>2016</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E42" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="G42" t="s">
-        <v>114</v>
-      </c>
-      <c r="H42">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H42" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B43">
         <v>2016</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E43" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="F43" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="G43" t="s">
-        <v>114</v>
-      </c>
-      <c r="H43">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B44">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>269</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>147</v>
+        <v>246</v>
       </c>
       <c r="E44" t="s">
-        <v>148</v>
+        <v>297</v>
       </c>
       <c r="F44" t="s">
-        <v>150</v>
+        <v>56</v>
       </c>
       <c r="G44" t="s">
-        <v>149</v>
-      </c>
-      <c r="H44">
+        <v>332</v>
+      </c>
+      <c r="H44" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>2015</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E45" t="s">
+        <v>297</v>
+      </c>
+      <c r="F45" t="s">
+        <v>239</v>
+      </c>
+      <c r="G45" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" t="s">
+        <v>34</v>
+      </c>
+      <c r="I45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>2015</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E46" t="s">
         <v>16</v>
       </c>
-      <c r="B45">
-        <v>2016</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="E45" t="s">
-        <v>110</v>
-      </c>
-      <c r="F45" t="s">
-        <v>111</v>
-      </c>
-      <c r="G45" t="s">
+      <c r="F46" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" t="s">
+        <v>332</v>
+      </c>
+      <c r="H46" t="s">
         <v>50</v>
       </c>
-      <c r="H45">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B46">
-        <v>2016</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="E46" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" t="s">
-        <v>128</v>
-      </c>
-      <c r="G46" t="s">
-        <v>105</v>
-      </c>
-      <c r="H46">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B47">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="F47" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="G47" t="s">
+        <v>332</v>
+      </c>
+      <c r="H47" t="s">
         <v>50</v>
       </c>
-      <c r="H47">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B48">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="F48" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="G48" t="s">
-        <v>105</v>
-      </c>
-      <c r="H48">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H48" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B49">
         <v>2015</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E49" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F49" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G49" t="s">
-        <v>50</v>
-      </c>
-      <c r="H49">
+        <v>332</v>
+      </c>
+      <c r="H49" t="s">
+        <v>5</v>
+      </c>
+      <c r="I49">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B50">
         <v>2015</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E50" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F50" t="s">
-        <v>239</v>
+        <v>4</v>
       </c>
       <c r="G50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H50">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H50" t="s">
+        <v>5</v>
+      </c>
+      <c r="I50">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B51">
         <v>2015</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>246</v>
+        <v>147</v>
       </c>
       <c r="E51" t="s">
-        <v>303</v>
+        <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="G51" t="s">
-        <v>5</v>
-      </c>
-      <c r="H51">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H51" t="s">
+        <v>29</v>
+      </c>
+      <c r="I51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B52">
         <v>2015</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E52" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="F52" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="G52" t="s">
-        <v>5</v>
-      </c>
-      <c r="H52">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>22</v>
+      </c>
+      <c r="H52" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B53">
         <v>2015</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
       <c r="E53" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F53" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="G53" t="s">
-        <v>50</v>
-      </c>
-      <c r="H53">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>332</v>
+      </c>
+      <c r="H53" t="s">
+        <v>37</v>
+      </c>
+      <c r="I53">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B54">
         <v>2015</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
       <c r="E54" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F54" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="G54" t="s">
-        <v>50</v>
-      </c>
-      <c r="H54">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B55">
-        <v>2015</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="E55" t="s">
-        <v>304</v>
-      </c>
-      <c r="F55" t="s">
-        <v>4</v>
-      </c>
-      <c r="G55" t="s">
-        <v>5</v>
-      </c>
-      <c r="H55">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B56">
-        <v>2015</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E56" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" t="s">
-        <v>12</v>
-      </c>
-      <c r="H56">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B57">
-        <v>2015</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E57" t="s">
-        <v>27</v>
-      </c>
-      <c r="F57" t="s">
-        <v>28</v>
-      </c>
-      <c r="G57" t="s">
-        <v>29</v>
-      </c>
-      <c r="H57">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B58">
-        <v>2015</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="E58" t="s">
-        <v>21</v>
-      </c>
-      <c r="F58" t="s">
-        <v>22</v>
-      </c>
-      <c r="G58" t="s">
-        <v>12</v>
-      </c>
-      <c r="H58">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B59">
-        <v>2015</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="E59" t="s">
-        <v>36</v>
-      </c>
-      <c r="F59" t="s">
-        <v>37</v>
-      </c>
-      <c r="G59" t="s">
+        <v>332</v>
+      </c>
+      <c r="H54" t="s">
         <v>40</v>
       </c>
-      <c r="H59">
+      <c r="I54">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B60">
-        <v>2015</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="E60" t="s">
-        <v>36</v>
-      </c>
-      <c r="F60" t="s">
-        <v>17</v>
-      </c>
-      <c r="G60" t="s">
-        <v>37</v>
-      </c>
-      <c r="H60">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:H60" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B19:H61">
-    <sortCondition descending="1" ref="B21:B61"/>
-    <sortCondition descending="1" ref="C21:C61"/>
+  <autoFilter ref="B1:I54" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:I64">
+    <sortCondition descending="1" ref="A5:A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>